<commit_message>
added plant bacteria comparison
</commit_message>
<xml_diff>
--- a/animals/animal_biomass_estimate.xlsx
+++ b/animals/animal_biomass_estimate.xlsx
@@ -443,7 +443,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.0896168300034035</v>
+        <v>0.08961683000340349</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -481,10 +481,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.667610883535102</v>
+        <v>0.6676108835351025</v>
       </c>
       <c r="C7">
-        <v>8.19778384931088</v>
+        <v>8.25174260997824</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -500,10 +500,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0.00734425384032944</v>
+        <v>0.007344253840329439</v>
       </c>
       <c r="C9">
-        <v>1.80611638932305</v>
+        <v>1.810927128263295</v>
       </c>
     </row>
     <row r="10" spans="1:3">

</xml_diff>

<commit_message>
add html for plants
</commit_message>
<xml_diff>
--- a/animals/animal_biomass_estimate.xlsx
+++ b/animals/animal_biomass_estimate.xlsx
@@ -484,7 +484,7 @@
         <v>0.667610883535102</v>
       </c>
       <c r="C7">
-        <v>8.26103681538425</v>
+        <v>8.30608554433884</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -503,7 +503,7 @@
         <v>0.00734425384032944</v>
       </c>
       <c r="C9">
-        <v>1.81026824322344</v>
+        <v>1.81092933001676</v>
       </c>
     </row>
     <row r="10" spans="1:3">

</xml_diff>